<commit_message>
Aktualisert status. Godkjenningsønsker og endringer sendt inn til arketyper.no V/Silje
</commit_message>
<xml_diff>
--- a/Arketyper_operasjonsplanlegging_status.xlsx
+++ b/Arketyper_operasjonsplanlegging_status.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="82">
   <si>
     <t>Type</t>
   </si>
@@ -109,9 +109,6 @@
 nb</t>
   </si>
   <si>
-    <t>Mangler DIPS endring</t>
-  </si>
-  <si>
     <t>ok  
 Endring: hastegrad lagt til</t>
   </si>
@@ -119,13 +116,6 @@
     <t>Problem diagnose</t>
   </si>
   <si>
-    <t>Må meldes til godkjening.</t>
-  </si>
-  <si>
-    <t>Må meldes til godkjenning.
-Må meldes endring.</t>
-  </si>
-  <si>
     <t>Evaluation</t>
   </si>
   <si>
@@ -146,18 +136,6 @@
   <si>
     <t>Ikke oppdatert med norsk versjon
 Bruk må endelig avklares internt</t>
-  </si>
-  <si>
-    <t>Må meldes til godkjening.
-Oppdatert versjon må importeres og tas i bruk</t>
-  </si>
-  <si>
-    <t>Må meldes til godkjening.
-Oppdatert versjon må importeres når oversettelsen er godkjent og tas i bruk.</t>
-  </si>
-  <si>
-    <t>Må meldes til godkjenning.
-Oppdatert versjon må importeres og tas i bruk</t>
   </si>
   <si>
     <t>Prosedyrerekvisisjon</t>
@@ -170,17 +148,6 @@
 Ønskes gjennomført innen</t>
   </si>
   <si>
-    <t>Mangler endringer fra DIPS</t>
-  </si>
-  <si>
-    <t>Må meldes til godkjenning.
-Ednring må synkroniseres med arketyper.no og sende på e-post til Silje.</t>
-  </si>
-  <si>
-    <t>Må meldes til godkjenning.
-Må importeres når oversettelsen i arketyper.no er godkjent.</t>
-  </si>
-  <si>
     <t>Ligger med egen oversettelse:( i ikke oppdatert versjon.</t>
   </si>
   <si>
@@ -290,13 +257,295 @@
 Må lastes opp i arketyper.no etter intern gjennomgang
 Må meldes til godkjenning
 Må oversettes til engelsk.</t>
+  </si>
+  <si>
+    <t>NYHA heart feilure classification</t>
+  </si>
+  <si>
+    <t>Skal den brukes?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Må meldes til godkjenning.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  ok </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Må importeres når oversettelsen i arketyper.no er godkjent.</t>
+    </r>
+  </si>
+  <si>
+    <t>meldt 05.02.15</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Må meldes til godkjenning.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  ok </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Må meldes til godkjenning.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  ok </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Oppdatert versjon må importeres når oversettelsen er godkjent og tas i bruk.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Må meldes til godkjenning.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  ok </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Oppdatert versjon må importeres og tas i bruk</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Må meldes til godkjenning</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.  ok </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Oppdatert versjon må importeres og tas i bruk</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Må meldes til godkjenning.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  ok </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Endring må synkroniseres med arketyper.no og sende på e-post til Silje.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- ok, sendt e-post til Silje 09.02</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Må meldes til godkjenning.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  ok </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Må meldes endring. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- ok, sendt e-post til Silje 09.02</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mangler DIPS endring </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Endring sendt 09.02.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mangler endringer fra DIPS - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Endring sendt 09.02.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,16 +576,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -611,39 +886,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -759,20 +1008,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1056,17 +1314,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.21875" style="2" customWidth="1"/>
     <col min="2" max="2" width="54.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="33.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
@@ -1074,41 +1332,38 @@
     <col min="8" max="16384" width="21.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="15" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:7" s="15" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-    </row>
-    <row r="2" spans="1:10" s="21" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+    </row>
+    <row r="2" spans="1:7" s="21" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>12</v>
@@ -1117,16 +1372,13 @@
         <v>13</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" s="25" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="25" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="35" t="s">
         <v>9</v>
       </c>
@@ -1142,17 +1394,14 @@
       <c r="E3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" s="30" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F3" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="30" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="26" t="s">
         <v>23</v>
       </c>
@@ -1160,33 +1409,30 @@
         <v>24</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>27</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>25</v>
@@ -1194,23 +1440,20 @@
       <c r="E5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" s="25" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="42" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="25" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="31"/>
       <c r="B6" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="33" t="s">
         <v>32</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>35</v>
       </c>
       <c r="D6" s="33" t="s">
         <v>25</v>
@@ -1218,25 +1461,22 @@
       <c r="E6" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="32" t="s">
-        <v>14</v>
+      <c r="F6" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="G6" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>25</v>
@@ -1244,22 +1484,22 @@
       <c r="E7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="21" t="s">
-        <v>14</v>
+      <c r="F7" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="18" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="18" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="32" t="s">
-        <v>36</v>
-      </c>
       <c r="C8" s="33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D8" s="33" t="s">
         <v>25</v>
@@ -1267,41 +1507,58 @@
       <c r="E8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="32" t="s">
-        <v>14</v>
+      <c r="F8" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="3" customFormat="1" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="36" t="s">
+      <c r="B10" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="E10" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="38" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1370,7 +1627,7 @@
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="11" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="18" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1428,7 +1685,7 @@
     <col min="8" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="39" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="40" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1456,467 +1713,467 @@
         <v>9</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="20"/>
       <c r="B3" s="4" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F3" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
       <c r="B4" s="4" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F4" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
       <c r="B5" s="4" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
       <c r="B6" s="4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F6" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="20"/>
       <c r="B7" s="4" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="20"/>
       <c r="B8" s="4" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F8" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="20"/>
       <c r="B9" s="4" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F9" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="31"/>
       <c r="B10" s="32" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F10" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F11" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="20"/>
       <c r="B12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>72</v>
-      </c>
       <c r="F12" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
       <c r="B13" s="4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F13" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="20"/>
       <c r="B14" s="4" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F14" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="20"/>
       <c r="B15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="24" t="s">
         <v>69</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="20"/>
       <c r="B16" s="4" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F16" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="31" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F17" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="22"/>
       <c r="B18" s="21" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F18" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="20"/>
       <c r="B19" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F19" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="20"/>
       <c r="B20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>71</v>
-      </c>
       <c r="E20" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F20" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="20"/>
       <c r="B21" s="4" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F21" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="20"/>
       <c r="B22" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="19" t="s">
-        <v>75</v>
-      </c>
       <c r="D22" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F22" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="31"/>
       <c r="B23" s="32" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F23" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Endret oppbyggingen, men ikke lagt inn definisjoner enda.
</commit_message>
<xml_diff>
--- a/Arketyper_operasjonsplanlegging_status.xlsx
+++ b/Arketyper_operasjonsplanlegging_status.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="81">
   <si>
     <t>Type</t>
   </si>
@@ -128,27 +128,10 @@
     <t>Anamnese</t>
   </si>
   <si>
-    <t>Ikke oppdatert med norsk versjon</t>
-  </si>
-  <si>
     <t>Funn ved klinisk undersøkelse</t>
   </si>
   <si>
-    <t>Ikke oppdatert med norsk versjon
-Bruk må endelig avklares internt</t>
-  </si>
-  <si>
     <t>Prosedyrerekvisisjon</t>
-  </si>
-  <si>
-    <t>OBS. Ligger med egen oversettelse og endringer og det finnes en aktulisert oversatt versjon uten våre endringer.
-Bruk må diskuteres internt
-Endringer: lagt til:
-Første dato for gjennomføring
-Ønskes gjennomført innen</t>
-  </si>
-  <si>
-    <t>Ligger med egen oversettelse:( i ikke oppdatert versjon.</t>
   </si>
   <si>
     <t xml:space="preserve">Må oversettes hvis den brukes.
@@ -156,15 +139,6 @@
 </t>
   </si>
   <si>
-    <t>Tilleggsprosedyre</t>
-  </si>
-  <si>
-    <t>Knivtid</t>
-  </si>
-  <si>
-    <t>Omsorgsnivå</t>
-  </si>
-  <si>
     <t>Ønsket anestesi</t>
   </si>
   <si>
@@ -232,10 +206,6 @@
   </si>
   <si>
     <t>ok i GIT
-satt opp til diskusjon i arketypeforum</t>
-  </si>
-  <si>
-    <t>mangler definsisjoner i GIT
 satt opp til diskusjon i arketypeforum</t>
   </si>
   <si>
@@ -539,6 +509,31 @@
       </rPr>
       <t xml:space="preserve"> Endring sendt 09.02.</t>
     </r>
+  </si>
+  <si>
+    <t>Tilleggsprosedyre - additional procedure code</t>
+  </si>
+  <si>
+    <t>Knivtid - surgery time</t>
+  </si>
+  <si>
+    <t>Omsorgsnivå - level of care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ok i GIT
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ok  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ok. 
+</t>
+  </si>
+  <si>
+    <t>ok
+Endring: lagt til to felt for ønsket tidspunkt for gjenomføring og tiddligst mulig dato for gjennomføring.</t>
   </si>
 </sst>
 </file>
@@ -597,7 +592,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -607,6 +602,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -892,7 +893,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1030,6 +1031,27 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1317,7 +1339,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1362,8 +1384,8 @@
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>37</v>
+      <c r="C2" s="49" t="s">
+        <v>79</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>12</v>
@@ -1372,10 +1394,10 @@
         <v>13</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="25" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1385,7 +1407,7 @@
       <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="50" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -1395,10 +1417,10 @@
         <v>15</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G3" s="41" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="30" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1408,20 +1430,20 @@
       <c r="B4" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="51" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1431,8 +1453,8 @@
       <c r="B5" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="23" t="s">
-        <v>26</v>
+      <c r="C5" s="47" t="s">
+        <v>78</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>25</v>
@@ -1441,10 +1463,10 @@
         <v>13</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G5" s="42" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="25" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1452,8 +1474,8 @@
       <c r="B6" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="33" t="s">
-        <v>32</v>
+      <c r="C6" s="47" t="s">
+        <v>78</v>
       </c>
       <c r="D6" s="33" t="s">
         <v>25</v>
@@ -1462,10 +1484,10 @@
         <v>13</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G6" s="34" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1475,8 +1497,8 @@
       <c r="B7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>32</v>
+      <c r="C7" s="47" t="s">
+        <v>78</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>25</v>
@@ -1485,10 +1507,10 @@
         <v>15</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="18" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1496,10 +1518,10 @@
         <v>30</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>78</v>
       </c>
       <c r="D8" s="33" t="s">
         <v>25</v>
@@ -1508,10 +1530,10 @@
         <v>15</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1519,10 +1541,10 @@
         <v>30</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="45" t="s">
-        <v>71</v>
+        <v>62</v>
+      </c>
+      <c r="C9" s="53" t="s">
+        <v>63</v>
       </c>
       <c r="D9" s="45" t="s">
         <v>12</v>
@@ -1537,27 +1559,27 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" s="3" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="35" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="C10" s="52" t="s">
+        <v>80</v>
       </c>
       <c r="D10" s="36" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G10" s="38" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1627,7 +1649,7 @@
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="18" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1670,7 +1692,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G23"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1713,190 +1735,190 @@
         <v>9</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>64</v>
+        <v>74</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>57</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="20"/>
       <c r="B3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>65</v>
+        <v>75</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>57</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F3" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
       <c r="B4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>66</v>
+        <v>76</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>77</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F4" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
       <c r="B5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>64</v>
+        <v>35</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>57</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
       <c r="B6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>66</v>
+        <v>36</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>77</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F6" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="20"/>
       <c r="B7" s="4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="20"/>
       <c r="B8" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F8" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="20"/>
       <c r="B9" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F9" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="31"/>
       <c r="B10" s="32" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F10" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -1904,276 +1926,276 @@
         <v>28</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F11" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="20"/>
       <c r="B12" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F12" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
       <c r="B13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="21" t="s">
         <v>56</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>63</v>
       </c>
       <c r="F13" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="20"/>
       <c r="B14" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F14" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="20"/>
       <c r="B15" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F15" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="20"/>
       <c r="B16" s="4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F16" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="31" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F17" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="22"/>
       <c r="B18" s="21" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F18" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="20"/>
       <c r="B19" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F19" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="20"/>
       <c r="B20" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F20" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="20"/>
       <c r="B21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>62</v>
-      </c>
       <c r="E21" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F21" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="20"/>
       <c r="B22" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F22" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="31"/>
       <c r="B23" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>66</v>
-      </c>
       <c r="D23" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F23" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
openEHR-EHR-OBSERVATION.body_mass_index.v1.adl: lastet oppgoskjent versjon fra akretyper.no openEHR-EHR-OBSERVATION.body_weight.v1.adl: lastet oppgoskjent versjon fra akretyper.no openEHR-EHR-OBSERVATION.height.v1.adl: lastet oppgoskjent versjon fra akretyper.no
Arketyper status - oppdatert status 16.02.15
</commit_message>
<xml_diff>
--- a/Arketyper_operasjonsplanlegging_status.xlsx
+++ b/Arketyper_operasjonsplanlegging_status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22968" windowHeight="9324" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Arketyper.no" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="79">
   <si>
     <t>Type</t>
   </si>
@@ -139,61 +139,25 @@
 </t>
   </si>
   <si>
-    <t>Ønsket anestesi</t>
-  </si>
-  <si>
-    <t>Ønsket helsepersonell</t>
-  </si>
-  <si>
-    <t>Tilleggsinformasjon kirurgi</t>
-  </si>
-  <si>
-    <t>Tilleggsinformasjon pasient</t>
-  </si>
-  <si>
-    <t>Hastegrad</t>
-  </si>
-  <si>
-    <t>Spesialutstyr</t>
-  </si>
-  <si>
-    <t>Operasjonsdetaljer</t>
-  </si>
-  <si>
     <t>Observasjon</t>
   </si>
   <si>
     <t>Høyde</t>
   </si>
   <si>
-    <t>Lengde</t>
-  </si>
-  <si>
     <t>Kroppsvekt</t>
   </si>
   <si>
     <t>Kroppsmasseindeks</t>
   </si>
   <si>
-    <t>ASA klassifikasjon helsetilstand</t>
-  </si>
-  <si>
     <t>Risikovurdering organ</t>
   </si>
   <si>
-    <t>Annen risikofaktor til kirurgi</t>
-  </si>
-  <si>
     <t>Medikamentbruk med betydning for inngrep og narkose</t>
   </si>
   <si>
     <t xml:space="preserve">Livsstilfaktor med betydening for inngrep og narkose </t>
-  </si>
-  <si>
-    <t>Annen risikofaktor til anestesi</t>
-  </si>
-  <si>
-    <t>Vurdering anestesirisiko</t>
   </si>
   <si>
     <t>Planlagt anestesi</t>
@@ -229,12 +193,12 @@
 Må oversettes til engelsk.</t>
   </si>
   <si>
-    <t>NYHA heart feilure classification</t>
-  </si>
-  <si>
     <t>Skal den brukes?</t>
   </si>
   <si>
+    <t>meldt 05.02.15</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -253,73 +217,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">  ok </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Må importeres når oversettelsen i arketyper.no er godkjent.</t>
-    </r>
-  </si>
-  <si>
-    <t>meldt 05.02.15</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Må meldes til godkjenning.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  ok </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Må meldes til godkjenning.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  ok </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Oppdatert versjon må importeres når oversettelsen er godkjent og tas i bruk.</t>
     </r>
   </si>
   <si>
@@ -511,15 +408,6 @@
     </r>
   </si>
   <si>
-    <t>Tilleggsprosedyre - additional procedure code</t>
-  </si>
-  <si>
-    <t>Knivtid - surgery time</t>
-  </si>
-  <si>
-    <t>Omsorgsnivå - level of care</t>
-  </si>
-  <si>
     <t xml:space="preserve">ok i GIT
 </t>
   </si>
@@ -528,19 +416,267 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">ok. 
-</t>
-  </si>
-  <si>
     <t>ok
 Endring: lagt til to felt for ønsket tidspunkt for gjenomføring og tiddligst mulig dato for gjennomføring.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tilleggsprosedyre  
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>additional procedure code</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Knivtid
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>surgery time</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Omsorgsnivå
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>level of care</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ønsket helsepersonell
+ID:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>required mediacal personell</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ønsket anestesi
+ID:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>anesthesia requested</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hastegrad
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>priority level</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tilleggsinformasjon pasient
+ID: a</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dditional information patient surgery</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tilleggsinformasjon kirurgi
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>additional information surgery</t>
+    </r>
+  </si>
+  <si>
+    <t>Spesialutstyr
+ID: spesialutstyr</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Operasjonsdetaljer
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>surgery details</t>
+    </r>
+  </si>
+  <si>
+    <t>NYHA heart failure classification</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Må meldes til godkjenning.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  ok </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Må importeres på nytt når oversettelsen i arketyper.no er godkjent.</t>
+    </r>
+  </si>
+  <si>
+    <t>ok. 
+Importert med foreløpig norsk oversettelse.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Må meldes til godkjenning.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  ok </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Oppdatert versjon må importeres på nytt når oversettelsen er godkjent og tas i bruk.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Vurdering anestesirisiko
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>risk assessment anesthesia</t>
+    </r>
+  </si>
+  <si>
+    <t>nb
+en</t>
+  </si>
+  <si>
+    <t>godkjent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -591,8 +727,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -608,6 +752,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -893,7 +1043,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1015,9 +1165,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1042,9 +1189,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1053,6 +1197,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1336,10 +1495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1354,7 +1513,7 @@
     <col min="8" max="16384" width="21.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="15" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="15" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1377,15 +1536,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="21" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="21" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="49" t="s">
-        <v>79</v>
+      <c r="C2" s="48" t="s">
+        <v>74</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>12</v>
@@ -1394,67 +1553,68 @@
         <v>13</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="25" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="25" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="41" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="30" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F3" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" s="30" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="26" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="49" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="47" t="s">
-        <v>78</v>
+      <c r="C5" s="46" t="s">
+        <v>60</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>25</v>
@@ -1463,19 +1623,21 @@
         <v>13</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="42" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="25" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="31"/>
+        <v>51</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="25" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="B6" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="47" t="s">
-        <v>78</v>
+      <c r="C6" s="48" t="s">
+        <v>74</v>
       </c>
       <c r="D6" s="33" t="s">
         <v>25</v>
@@ -1484,21 +1646,21 @@
         <v>13</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="G6" s="34" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="47" t="s">
-        <v>78</v>
+      <c r="C7" s="46" t="s">
+        <v>60</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>25</v>
@@ -1507,79 +1669,138 @@
         <v>15</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="18" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="1" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="24"/>
+    </row>
+    <row r="9" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="20"/>
+      <c r="B9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="24"/>
+    </row>
+    <row r="10" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="20"/>
+      <c r="B10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="24"/>
+    </row>
+    <row r="11" spans="1:8" s="18" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B11" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" s="33" t="s">
+      <c r="C11" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E11" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G8" s="34" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="43" t="s">
+      <c r="F11" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" s="45" t="s">
+      <c r="B12" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E12" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F12" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="46" t="s">
+      <c r="G12" s="45" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="35" t="s">
+    <row r="13" spans="1:8" s="3" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B13" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="36" t="s">
+      <c r="C13" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G10" s="38" t="s">
-        <v>70</v>
+      <c r="E13" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="38" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1689,10 +1910,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1734,471 +1955,325 @@
       <c r="A2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="47" t="s">
-        <v>57</v>
+      <c r="B2" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>45</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="20"/>
-      <c r="B3" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>57</v>
+      <c r="B3" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>45</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F3" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="48" t="s">
-        <v>77</v>
+      <c r="B4" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>59</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F4" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
-      <c r="B5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="47" t="s">
-        <v>57</v>
+      <c r="B5" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>45</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
-      <c r="B6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="48" t="s">
-        <v>77</v>
+      <c r="B6" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>59</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F6" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="20"/>
-      <c r="B7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>58</v>
+      <c r="B7" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>45</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="20"/>
-      <c r="B8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>58</v>
+      <c r="B8" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>45</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F8" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="20"/>
-      <c r="B9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>58</v>
+      <c r="B9" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>45</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F9" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="31"/>
-      <c r="B10" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>58</v>
+      <c r="B10" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>45</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F10" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>58</v>
+      <c r="B11" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>45</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F11" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="20"/>
       <c r="B12" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F12" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="20"/>
-      <c r="B13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
-      <c r="B14" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
-      <c r="B15" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
+    </row>
+    <row r="16" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="31" t="s">
+        <v>35</v>
+      </c>
       <c r="B16" s="4" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F16" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="20"/>
+      <c r="B17" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>55</v>
-      </c>
       <c r="E17" s="21" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F17" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
-      <c r="B18" s="21" t="s">
+      <c r="A18" s="20"/>
+      <c r="B18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="21" t="s">
         <v>44</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>56</v>
       </c>
       <c r="F18" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
-      <c r="B19" s="4" t="s">
-        <v>45</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="31"/>
+      <c r="B19" s="32" t="s">
+        <v>41</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F19" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
-      <c r="B21" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
-      <c r="B22" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="31"/>
-      <c r="B23" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="24" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Oppdatert status. Ny gjennomgagn av alle arketypene. Dobbeltsjekk på skrivefeil, occurancy etc. openEHR-EHR-CLUSTER.anesthesia_type.v1.adl - erstattes av openEHR-EHR-CLUSTER.anesthesia_requested.v1.adl. openEHR-EHR-CLUSTER.spesialutstyr.v1.adl - gitt nytt navn: openEHR-EHR-CLUSTER.special_requirements_surgery.v1.adl openEHR-EHR-EVALUATION.planlagt_anestesi.v1.adl: omgjort til obervation. ny arketype heter openEHR-EHR-OBSERVATION.planned_anesthesia.v1.adl
</commit_message>
<xml_diff>
--- a/Arketyper_operasjonsplanlegging_status.xlsx
+++ b/Arketyper_operasjonsplanlegging_status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22968" windowHeight="9324" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12288" windowHeight="5652" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arketyper.no" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="79">
   <si>
     <t>Type</t>
   </si>
@@ -361,10 +361,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">ok i GIT
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">ok  
 </t>
   </si>
@@ -507,10 +503,6 @@
       </rPr>
       <t>additional information surgery</t>
     </r>
-  </si>
-  <si>
-    <t>Spesialutstyr
-ID: spesialutstyr</t>
   </si>
   <si>
     <r>
@@ -648,12 +640,6 @@
 Må oversettes til engelsk.</t>
   </si>
   <si>
-    <t>Evalutaion: planlagt anestesi må slettes
-Må lastes opp i arketyper.no etter intern gjennomgang
-Må meldes til godkjenning
-Må oversettes til engelsk.</t>
-  </si>
-  <si>
     <t>Koder må legges inn.
 Må lastes opp i arketyper.no etter intern gjennomgang
 Må meldes til godkjenning
@@ -790,8 +776,50 @@
     </r>
   </si>
   <si>
-    <t>Medikamenter ved kirurgi
-ID: medicine surgery</t>
+    <r>
+      <t xml:space="preserve">Medikamenter ved kirurgi
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>medicine surgery</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Spesielle behov kirurgi
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>special requirements surgery</t>
+    </r>
+  </si>
+  <si>
+    <t>ok i GIT
+klar til intern gjennomgang</t>
+  </si>
+  <si>
+    <t>ok i GIT
+må diskuteres i arketypeforum. Trenger vi denne?</t>
+  </si>
+  <si>
+    <t>ok i GIT
+mangler protocol, participation etc.</t>
   </si>
 </sst>
 </file>
@@ -1165,7 +1193,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1284,9 +1312,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1317,10 +1342,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1607,7 +1641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="B4" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -1653,8 +1687,8 @@
       <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="41" t="s">
-        <v>61</v>
+      <c r="C2" s="40" t="s">
+        <v>59</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>12</v>
@@ -1666,29 +1700,29 @@
         <v>38</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="18" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="47" t="s">
         <v>39</v>
       </c>
       <c r="H3" s="4"/>
@@ -1700,7 +1734,7 @@
       <c r="B4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="21" t="s">
@@ -1724,7 +1758,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>19</v>
@@ -1746,8 +1780,8 @@
       <c r="B6" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="41" t="s">
-        <v>61</v>
+      <c r="C6" s="40" t="s">
+        <v>59</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>19</v>
@@ -1759,7 +1793,7 @@
         <v>38</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1770,7 +1804,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>19</v>
@@ -1793,16 +1827,16 @@
         <v>29</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="49" t="s">
-        <v>65</v>
+      <c r="F8" s="48" t="s">
+        <v>63</v>
       </c>
       <c r="G8" s="17"/>
     </row>
@@ -1812,16 +1846,16 @@
         <v>30</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="49" t="s">
-        <v>65</v>
+      <c r="F9" s="48" t="s">
+        <v>63</v>
       </c>
       <c r="G9" s="17"/>
     </row>
@@ -1831,16 +1865,16 @@
         <v>31</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="49" t="s">
-        <v>65</v>
+      <c r="F10" s="48" t="s">
+        <v>63</v>
       </c>
       <c r="G10" s="17"/>
     </row>
@@ -1852,7 +1886,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>19</v>
@@ -1872,9 +1906,9 @@
         <v>24</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="43" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="37" t="s">
@@ -1897,8 +1931,8 @@
       <c r="B13" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="43" t="s">
-        <v>48</v>
+      <c r="C13" s="42" t="s">
+        <v>47</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>19</v>
@@ -1923,15 +1957,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" style="53" customWidth="1"/>
     <col min="4" max="4" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -1946,7 +1980,7 @@
       <c r="B1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="51" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -1967,10 +2001,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>32</v>
@@ -1988,10 +2022,10 @@
     <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
       <c r="B3" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="40" t="s">
-        <v>34</v>
+        <v>49</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>76</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>32</v>
@@ -2009,10 +2043,10 @@
     <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>
       <c r="B4" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>46</v>
+        <v>50</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>76</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>32</v>
@@ -2030,10 +2064,10 @@
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="13"/>
       <c r="B5" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>32</v>
@@ -2051,10 +2085,10 @@
     <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="13"/>
       <c r="B6" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>46</v>
+        <v>51</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>76</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>32</v>
@@ -2072,10 +2106,10 @@
     <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>32</v>
@@ -2093,10 +2127,10 @@
     <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
       <c r="B8" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>32</v>
@@ -2114,10 +2148,10 @@
     <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="13"/>
       <c r="B9" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>34</v>
+        <v>53</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>77</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>32</v>
@@ -2132,100 +2166,100 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" s="11" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="24"/>
       <c r="B10" s="26" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="C10" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="50" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="24"/>
+      <c r="B11" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="11" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="50" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D13" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E13" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F13" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="11" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="51" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="52" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="50"/>
-      <c r="B13" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="52" t="s">
-        <v>36</v>
+      <c r="G13" s="17" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="50"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="52" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="36" t="s">
@@ -2237,17 +2271,17 @@
       <c r="F14" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="52" t="s">
+      <c r="G14" s="50" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="50"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>34</v>
+        <v>69</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>78</v>
       </c>
       <c r="D15" s="36" t="s">
         <v>32</v>
@@ -2258,16 +2292,16 @@
       <c r="F15" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="52" t="s">
+      <c r="G15" s="50" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="50"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="52" t="s">
         <v>34</v>
       </c>
       <c r="D16" s="36" t="s">
@@ -2279,17 +2313,17 @@
       <c r="F16" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="52" t="s">
+      <c r="G16" s="50" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="50"/>
+      <c r="A17" s="49"/>
       <c r="B17" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="39" t="s">
-        <v>34</v>
+        <v>71</v>
+      </c>
+      <c r="C17" s="54" t="s">
+        <v>78</v>
       </c>
       <c r="D17" s="36" t="s">
         <v>32</v>
@@ -2300,37 +2334,37 @@
       <c r="F17" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="52" t="s">
+      <c r="G17" s="50" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="50"/>
-      <c r="B18" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="14" t="s">
+    <row r="18" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="49"/>
+      <c r="B18" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="17" t="s">
-        <v>67</v>
+      <c r="G18" s="50" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="39" t="s">
+      <c r="A19" s="49"/>
+      <c r="B19" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="52" t="s">
         <v>34</v>
       </c>
       <c r="D19" s="14" t="s">
@@ -2343,16 +2377,16 @@
         <v>14</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>34</v>
+        <v>64</v>
+      </c>
+      <c r="C20" s="54" t="s">
+        <v>78</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>32</v>
@@ -2367,24 +2401,24 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="11" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="24"/>
-      <c r="B21" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="51" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="36" t="s">
+    <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="13"/>
+      <c r="B21" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="36" t="s">
+      <c r="E21" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="36" t="s">
+      <c r="F21" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="52" t="s">
+      <c r="G21" s="17" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Siste gjennomgang av arketyper, retting av skrivefeil, ssjekket occurancy etc. openEHR-EHR-EVALUATION.adverse_reaction_fhir.v1.adl: lastet opp med foreløpig norsk oversettelse fra arketyper.no openEHR-EHR-EVALUATION.surgery_details.v1.adl: erstattes av openEHR-EHR-OBSERVATION.surgery_details.v1.adl openEHR-EHR-EVALUATION.vurdering_anestesirisiko.v1.adl: gitt nytt navn: openEHR-EHR-OBSERVATION.risk_assessment_anesthesia.v1.adl openEHR-EHR-OBSERVATION.hypersensitivity_reaction.v1.adl: kladd, startet på overfølsomhetreakjoner før jeg så at det finnes noe i arketyper.no
</commit_message>
<xml_diff>
--- a/Arketyper_operasjonsplanlegging_status.xlsx
+++ b/Arketyper_operasjonsplanlegging_status.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="78">
   <si>
     <t>Type</t>
   </si>
@@ -130,10 +130,6 @@
   </si>
   <si>
     <t>Ikke lastet opp</t>
-  </si>
-  <si>
-    <t>ok i GIT
-satt opp til diskusjon i arketypeforum</t>
   </si>
   <si>
     <t>Må lastes opp i arketyper.no etter intern gjennomgang
@@ -634,18 +630,6 @@
     </r>
   </si>
   <si>
-    <t>Evalutaion: vurdering anestesirisiko må slettes
-Må lastes opp i arketyper.no etter intern gjennomgang
-Må meldes til godkjenning
-Må oversettes til engelsk.</t>
-  </si>
-  <si>
-    <t>Koder må legges inn.
-Må lastes opp i arketyper.no etter intern gjennomgang
-Må meldes til godkjenning
-Må oversettes til engelsk.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Organstatus evaluering kirurgi
 ID: </t>
@@ -698,6 +682,110 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Spesifikke risikofaktorer anestesi
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>specific risk factors ansthesia</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Annen risikofaktor anesthesi
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>other risk factors anesthesia</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Risikofaktor medisiner kirurgi
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>risk factor medicine surgery</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Medikamenter ved kirurgi
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>medicine surgery</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Spesielle behov kirurgi
+ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>special requirements surgery</t>
+    </r>
+  </si>
+  <si>
+    <t>ok i GIT
+klar til intern gjennomgang</t>
+  </si>
+  <si>
+    <t>ok i GIT
+må diskuteres i arketypeforum. Trenger vi denne?</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Risikofaktor andre organer anestesi
 ID: </t>
     </r>
@@ -710,116 +798,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>risk factor lungs anesthesia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Spesifikke risikofaktorer anestesi
-ID: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>specific risk factors ansthesia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Annen risikofaktor anesthesi
-ID: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>other risk factors anesthesia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Risikofaktor medisiner kirurgi
-ID: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>risk factor medicine surgery</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Medikamenter ved kirurgi
-ID: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>medicine surgery</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Spesielle behov kirurgi
-ID: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>special requirements surgery</t>
-    </r>
-  </si>
-  <si>
-    <t>ok i GIT
-klar til intern gjennomgang</t>
-  </si>
-  <si>
-    <t>ok i GIT
-må diskuteres i arketypeforum. Trenger vi denne?</t>
-  </si>
-  <si>
-    <t>ok i GIT
-mangler protocol, participation etc.</t>
+      <t>risk factor other organs anesthesia</t>
+    </r>
+  </si>
+  <si>
+    <t>Må diskuteres internt og nasjonalt
+Ligger i arketyper.no men passer ikke:(</t>
+  </si>
+  <si>
+    <t>Usikker</t>
+  </si>
+  <si>
+    <t>Overfølsomhetsreaksjoner/Allergier</t>
   </si>
 </sst>
 </file>
@@ -886,7 +876,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -911,8 +901,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1187,13 +1183,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1321,9 +1365,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1348,14 +1389,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1641,8 +1703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1688,7 +1750,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>12</v>
@@ -1697,33 +1759,33 @@
         <v>13</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="18" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="46" t="s">
         <v>38</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="18" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="47" t="s">
-        <v>39</v>
       </c>
       <c r="H3" s="4"/>
     </row>
@@ -1741,13 +1803,13 @@
         <v>19</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1758,7 +1820,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>19</v>
@@ -1767,10 +1829,10 @@
         <v>13</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="34" t="s">
         <v>38</v>
-      </c>
-      <c r="G5" s="34" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="18" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1781,7 +1843,7 @@
         <v>23</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>19</v>
@@ -1790,10 +1852,10 @@
         <v>13</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1804,7 +1866,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>19</v>
@@ -1813,10 +1875,10 @@
         <v>15</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1827,16 +1889,16 @@
         <v>29</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="48" t="s">
-        <v>63</v>
+      <c r="F8" s="47" t="s">
+        <v>62</v>
       </c>
       <c r="G8" s="17"/>
     </row>
@@ -1846,16 +1908,16 @@
         <v>30</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="48" t="s">
-        <v>63</v>
+      <c r="F9" s="47" t="s">
+        <v>62</v>
       </c>
       <c r="G9" s="17"/>
     </row>
@@ -1865,16 +1927,16 @@
         <v>31</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="48" t="s">
-        <v>63</v>
+      <c r="F10" s="47" t="s">
+        <v>62</v>
       </c>
       <c r="G10" s="17"/>
     </row>
@@ -1886,7 +1948,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>19</v>
@@ -1895,10 +1957,10 @@
         <v>15</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1906,10 +1968,10 @@
         <v>24</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="43" t="s">
-        <v>37</v>
+        <v>56</v>
+      </c>
+      <c r="C12" s="53" t="s">
+        <v>36</v>
       </c>
       <c r="D12" s="37" t="s">
         <v>12</v>
@@ -1932,19 +1994,19 @@
         <v>27</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>19</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1955,17 +2017,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="53" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" style="51" customWidth="1"/>
     <col min="4" max="4" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -1980,7 +2042,7 @@
       <c r="B1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="50" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -2001,10 +2063,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>32</v>
@@ -2016,16 +2078,16 @@
         <v>14</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
       <c r="B3" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>32</v>
@@ -2037,16 +2099,16 @@
         <v>14</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>
       <c r="B4" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>32</v>
@@ -2058,16 +2120,16 @@
         <v>14</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="13"/>
       <c r="B5" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>32</v>
@@ -2079,16 +2141,16 @@
         <v>14</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="13"/>
       <c r="B6" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>32</v>
@@ -2100,16 +2162,16 @@
         <v>14</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>32</v>
@@ -2121,16 +2183,16 @@
         <v>14</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
       <c r="B8" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>32</v>
@@ -2142,16 +2204,16 @@
         <v>14</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="13"/>
       <c r="B9" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="54" t="s">
-        <v>77</v>
+        <v>52</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>73</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>32</v>
@@ -2163,16 +2225,16 @@
         <v>14</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="11" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="24"/>
       <c r="B10" s="26" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D10" s="36" t="s">
         <v>32</v>
@@ -2183,17 +2245,17 @@
       <c r="F10" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="50" t="s">
-        <v>36</v>
+      <c r="G10" s="49" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="24"/>
       <c r="B11" s="26" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>32</v>
@@ -2205,18 +2267,18 @@
         <v>14</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="11" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="35" t="s">
-        <v>22</v>
+      <c r="A12" s="48" t="s">
+        <v>28</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D12" s="36" t="s">
         <v>32</v>
@@ -2227,19 +2289,17 @@
       <c r="F12" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="50" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="49" t="s">
-        <v>28</v>
-      </c>
+      <c r="G12" s="49" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="48"/>
       <c r="B13" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="52" t="s">
-        <v>34</v>
+        <v>64</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>72</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>32</v>
@@ -2251,16 +2311,16 @@
         <v>14</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="49"/>
+      <c r="A14" s="48"/>
       <c r="B14" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="52" t="s">
-        <v>34</v>
+        <v>65</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>72</v>
       </c>
       <c r="D14" s="36" t="s">
         <v>32</v>
@@ -2271,17 +2331,17 @@
       <c r="F14" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="50" t="s">
-        <v>36</v>
+      <c r="G14" s="49" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="49"/>
+      <c r="A15" s="48"/>
       <c r="B15" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="54" t="s">
-        <v>78</v>
+        <v>66</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>72</v>
       </c>
       <c r="D15" s="36" t="s">
         <v>32</v>
@@ -2292,17 +2352,17 @@
       <c r="F15" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="50" t="s">
-        <v>36</v>
+      <c r="G15" s="49" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="49"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="52" t="s">
-        <v>34</v>
+        <v>74</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>72</v>
       </c>
       <c r="D16" s="36" t="s">
         <v>32</v>
@@ -2313,17 +2373,17 @@
       <c r="F16" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="50" t="s">
-        <v>36</v>
+      <c r="G16" s="49" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="49"/>
+      <c r="A17" s="48"/>
       <c r="B17" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="54" t="s">
-        <v>78</v>
+        <v>67</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>72</v>
       </c>
       <c r="D17" s="36" t="s">
         <v>32</v>
@@ -2334,17 +2394,17 @@
       <c r="F17" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="50" t="s">
-        <v>36</v>
+      <c r="G17" s="49" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="49"/>
+      <c r="A18" s="48"/>
       <c r="B18" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="39" t="s">
         <v>72</v>
-      </c>
-      <c r="C18" s="54" t="s">
-        <v>78</v>
       </c>
       <c r="D18" s="36" t="s">
         <v>32</v>
@@ -2355,17 +2415,17 @@
       <c r="F18" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="50" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="49"/>
+      <c r="G18" s="49" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="48"/>
       <c r="B19" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="52" t="s">
-        <v>34</v>
+        <v>60</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>72</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>32</v>
@@ -2377,16 +2437,16 @@
         <v>14</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="15"/>
       <c r="B20" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="54" t="s">
-        <v>78</v>
+        <v>63</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>72</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>32</v>
@@ -2398,28 +2458,39 @@
         <v>14</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
-      <c r="B21" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="54" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" s="14" t="s">
+      <c r="A21" s="54"/>
+      <c r="B21" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="17" t="s">
-        <v>36</v>
+      <c r="G21" s="58" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="59" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arketyper_operasjonsplanlegging_status.xlsx: ny oppdatert status openEHR-EHR-OBSERVATION.nyha_heart_failure_score.v1.adl: lastet opp fra arketyper.no med forleøpig norsk oversettelse. openEHR-EHR-OBSERVATION.planned_anesthesia.v1.adl: gitt norsk navn openEHR-EHR-OBSERVATION.risk_assessment_anesthesia.v1.adl: lagt til ASA
</commit_message>
<xml_diff>
--- a/Arketyper_operasjonsplanlegging_status.xlsx
+++ b/Arketyper_operasjonsplanlegging_status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12288" windowHeight="5652" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12288" windowHeight="5652"/>
   </bookViews>
   <sheets>
     <sheet name="Arketyper.no" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="79">
   <si>
     <t>Type</t>
   </si>
@@ -810,6 +810,9 @@
   </si>
   <si>
     <t>Overfølsomhetsreaksjoner/Allergier</t>
+  </si>
+  <si>
+    <t>Blodtrykk</t>
   </si>
 </sst>
 </file>
@@ -1237,7 +1240,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1417,6 +1420,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1701,10 +1716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1922,90 +1937,108 @@
       <c r="G9" s="17"/>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="54"/>
+      <c r="B10" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="47" t="s">
+      <c r="F10" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="17"/>
-    </row>
-    <row r="11" spans="1:8" s="11" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="39" t="s">
+      <c r="G10" s="58"/>
+    </row>
+    <row r="11" spans="1:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="25" t="s">
+      <c r="D11" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F11" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="44"/>
+    </row>
+    <row r="12" spans="1:8" s="11" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="35" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="49" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C13" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D13" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E13" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G13" s="38" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="28" t="s">
+    <row r="14" spans="1:8" s="3" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B14" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C14" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D14" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E14" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F14" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G14" s="31" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2019,8 +2052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Laget ny mappe "surgery" for operasjonsplanleggingen. Flyttet nye templates dit.
</commit_message>
<xml_diff>
--- a/Arketyper_operasjonsplanlegging_status.xlsx
+++ b/Arketyper_operasjonsplanlegging_status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12288" windowHeight="5652"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12288" windowHeight="5652" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arketyper.no" sheetId="1" r:id="rId1"/>
@@ -911,7 +911,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1234,13 +1234,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1323,115 +1334,118 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1716,10 +1730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1758,13 +1772,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="14" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="28" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="36" t="s">
         <v>58</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -1781,25 +1795,25 @@
       </c>
     </row>
     <row r="3" spans="1:8" s="18" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="41" t="s">
         <v>38</v>
       </c>
       <c r="H3" s="4"/>
@@ -1811,7 +1825,7 @@
       <c r="B4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="37" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="21" t="s">
@@ -1834,7 +1848,7 @@
       <c r="B5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="35" t="s">
         <v>45</v>
       </c>
       <c r="D5" s="16" t="s">
@@ -1846,7 +1860,7 @@
       <c r="F5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="G5" s="30" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1857,7 +1871,7 @@
       <c r="B6" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="36" t="s">
         <v>58</v>
       </c>
       <c r="D6" s="26" t="s">
@@ -1880,7 +1894,7 @@
       <c r="B7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="35" t="s">
         <v>45</v>
       </c>
       <c r="D7" s="16" t="s">
@@ -1903,7 +1917,7 @@
       <c r="B8" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="35" t="s">
         <v>45</v>
       </c>
       <c r="D8" s="16" t="s">
@@ -1912,7 +1926,7 @@
       <c r="E8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="47" t="s">
+      <c r="F8" s="42" t="s">
         <v>62</v>
       </c>
       <c r="G8" s="17"/>
@@ -1922,7 +1936,7 @@
       <c r="B9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="35" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="16" t="s">
@@ -1931,35 +1945,35 @@
       <c r="E9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="47" t="s">
+      <c r="F9" s="42" t="s">
         <v>62</v>
       </c>
       <c r="G9" s="17"/>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="54"/>
-      <c r="B10" s="62" t="s">
+      <c r="A10" s="49"/>
+      <c r="B10" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="64" t="s">
+      <c r="F10" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="58"/>
+      <c r="G10" s="53"/>
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="51" t="s">
         <v>45</v>
       </c>
       <c r="D11" s="12" t="s">
@@ -1968,45 +1982,45 @@
       <c r="E11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="61" t="s">
+      <c r="F11" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="44"/>
+      <c r="G11" s="39"/>
     </row>
     <row r="12" spans="1:8" s="11" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="32" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="49" t="s">
+      <c r="G12" s="44" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="53" t="s">
+      <c r="C13" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="33" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="26" t="s">
@@ -2015,32 +2029,41 @@
       <c r="F13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="38" t="s">
+      <c r="G13" s="34" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="3" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="28" t="s">
+    <row r="14" spans="1:8" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="64" t="s">
         <v>41</v>
       </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="65"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="64"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2052,15 +2075,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="51" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" style="46" customWidth="1"/>
     <col min="4" max="4" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -2068,14 +2091,14 @@
     <col min="8" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="33" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="29" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="45" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -2098,7 +2121,7 @@
       <c r="B2" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="35" t="s">
         <v>72</v>
       </c>
       <c r="D2" s="14" t="s">
@@ -2119,7 +2142,7 @@
       <c r="B3" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="35" t="s">
         <v>72</v>
       </c>
       <c r="D3" s="14" t="s">
@@ -2140,7 +2163,7 @@
       <c r="B4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="35" t="s">
         <v>72</v>
       </c>
       <c r="D4" s="14" t="s">
@@ -2161,7 +2184,7 @@
       <c r="B5" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="35" t="s">
         <v>72</v>
       </c>
       <c r="D5" s="14" t="s">
@@ -2182,7 +2205,7 @@
       <c r="B6" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="35" t="s">
         <v>72</v>
       </c>
       <c r="D6" s="14" t="s">
@@ -2203,7 +2226,7 @@
       <c r="B7" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="35" t="s">
         <v>72</v>
       </c>
       <c r="D7" s="14" t="s">
@@ -2224,7 +2247,7 @@
       <c r="B8" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="35" t="s">
         <v>72</v>
       </c>
       <c r="D8" s="14" t="s">
@@ -2245,7 +2268,7 @@
       <c r="B9" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="47" t="s">
         <v>73</v>
       </c>
       <c r="D9" s="14" t="s">
@@ -2266,19 +2289,19 @@
       <c r="B10" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E10" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="36" t="s">
+      <c r="F10" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="49" t="s">
+      <c r="G10" s="44" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2287,7 +2310,7 @@
       <c r="B11" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="35" t="s">
         <v>72</v>
       </c>
       <c r="D11" s="14" t="s">
@@ -2304,34 +2327,34 @@
       </c>
     </row>
     <row r="12" spans="1:7" s="11" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="36" t="s">
+      <c r="F12" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="49" t="s">
+      <c r="G12" s="44" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="48"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="35" t="s">
         <v>72</v>
       </c>
       <c r="D13" s="14" t="s">
@@ -2348,116 +2371,116 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="48"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="36" t="s">
+      <c r="F14" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="49" t="s">
+      <c r="G14" s="44" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="48"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="E15" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="36" t="s">
+      <c r="F15" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="49" t="s">
+      <c r="G15" s="44" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="48"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="36" t="s">
+      <c r="F16" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="49" t="s">
+      <c r="G16" s="44" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="48"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="36" t="s">
+      <c r="F17" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="49" t="s">
+      <c r="G17" s="44" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="48"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="D18" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="36" t="s">
+      <c r="E18" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="36" t="s">
+      <c r="F18" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="49" t="s">
+      <c r="G18" s="44" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="48"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="35" t="s">
         <v>72</v>
       </c>
       <c r="D19" s="14" t="s">
@@ -2478,7 +2501,7 @@
       <c r="B20" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="39" t="s">
+      <c r="C20" s="35" t="s">
         <v>72</v>
       </c>
       <c r="D20" s="14" t="s">
@@ -2495,34 +2518,34 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
-      <c r="B21" s="55" t="s">
+      <c r="A21" s="49"/>
+      <c r="B21" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="56" t="s">
+      <c r="C21" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="57" t="s">
+      <c r="D21" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="57" t="s">
+      <c r="E21" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="57" t="s">
+      <c r="F21" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="58" t="s">
+      <c r="G21" s="53" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="60" t="s">
+      <c r="A22" s="55" t="s">
         <v>76</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C22" s="59" t="s">
+      <c r="C22" s="54" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>